<commit_message>
Added chart info on OVERALL STUDENT PERFORMANCE FOR SUBJECT ON A TEST TYPE SECTION
</commit_message>
<xml_diff>
--- a/content/StudentResult_Science.xlsx
+++ b/content/StudentResult_Science.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adiza\Desktop\Streamlit-Test\ASSESSLY\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0738B6E-57D1-46F7-8100-07418FF32EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBA9A46-9182-41F4-9DF0-9F6227BD9468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{77A4484A-74D5-462C-9AEB-01A894CB0349}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{77A4484A-74D5-462C-9AEB-01A894CB0349}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CE4C3B-C0D6-4BED-AB94-292F80034206}">
   <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,27 +887,27 @@
       </c>
       <c r="C2" s="1">
         <f ca="1">RANDBETWEEN(50,100)</f>
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">RANDBETWEEN(50,100)</f>
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">RANDBETWEEN(50,100)</f>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1">
         <f ca="1">RANDBETWEEN(50,100)</f>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="1">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1">
         <f ca="1">RANDBETWEEN(70,100)</f>
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -919,27 +919,27 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:F66" ca="1" si="0">RANDBETWEEN(50,100)</f>
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G66" ca="1" si="1">RANDBETWEEN(1,20)</f>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H66" ca="1" si="2">RANDBETWEEN(70,100)</f>
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,27 +951,27 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -983,27 +983,27 @@
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,27 +1015,27 @@
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
-      <c r="F6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>65</v>
-      </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,27 +1047,27 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,27 +1079,27 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1111,15 +1111,15 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1127,11 +1127,11 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1143,27 +1143,27 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1175,27 +1175,27 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1207,27 +1207,27 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1239,27 +1239,27 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1275,23 +1275,23 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1303,27 +1303,27 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1367,27 +1367,27 @@
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1399,27 +1399,27 @@
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,27 +1431,27 @@
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1463,27 +1463,27 @@
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>79</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1495,27 +1495,27 @@
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1527,27 +1527,27 @@
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>83</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
       <c r="E22" s="1">
         <f t="shared" ca="1" si="0"/>
         <v>83</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1559,27 +1559,27 @@
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>90</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1591,27 +1591,27 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>73</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1623,27 +1623,27 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>79</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,27 +1655,27 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1687,27 +1687,27 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>75</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1719,27 +1719,27 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1751,27 +1751,27 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,27 +1783,27 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1815,27 +1815,27 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1847,27 +1847,27 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>77</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>92</v>
-      </c>
-      <c r="G32" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="H32" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1879,27 +1879,27 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>72</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="G33" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="H33" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1911,19 +1911,19 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,27 +1943,27 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1975,27 +1975,27 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2007,27 +2007,27 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2039,27 +2039,27 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,27 +2071,27 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,27 +2103,27 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2135,27 +2135,27 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2167,27 +2167,27 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>85</v>
       </c>
-      <c r="D42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>73</v>
-      </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2199,27 +2199,27 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2231,27 +2231,27 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2263,15 +2263,15 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2279,11 +2279,11 @@
       </c>
       <c r="G45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2295,7 +2295,7 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2303,15 +2303,15 @@
       </c>
       <c r="E46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2327,27 +2327,27 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2359,27 +2359,27 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2391,27 +2391,27 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2423,27 +2423,27 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" ca="1" si="2"/>
         <v>100</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="E50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="F50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="G50" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="H50" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2463,19 +2463,19 @@
       </c>
       <c r="E51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,27 +2487,27 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H52" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2519,19 +2519,19 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" ca="1" si="1"/>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="H53" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2551,27 +2551,27 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H54" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2583,27 +2583,27 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2615,27 +2615,27 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H56" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2647,27 +2647,27 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H57" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,27 +2679,27 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="D58" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>92</v>
       </c>
-      <c r="E58" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="F58" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
-      </c>
       <c r="G58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H58" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2711,27 +2711,27 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H59" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2743,27 +2743,27 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F60" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>88</v>
       </c>
-      <c r="D60" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="E60" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="F60" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>85</v>
-      </c>
       <c r="G60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H60" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2775,27 +2775,27 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="G61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H61" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2807,15 +2807,15 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2823,11 +2823,11 @@
       </c>
       <c r="G62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H62" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2839,27 +2839,27 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H63" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2871,27 +2871,27 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H64" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2903,27 +2903,27 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H65" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2935,23 +2935,23 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" ref="F66:F126" ca="1" si="3">RANDBETWEEN(50,100)</f>
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H66" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -2967,27 +2967,27 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" ref="C67:E126" ca="1" si="4">RANDBETWEEN(50,100)</f>
+        <v>77</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="F67" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>79</v>
-      </c>
-      <c r="D67" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>77</v>
-      </c>
-      <c r="E67" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="F67" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>62</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" ref="G67:G126" ca="1" si="5">RANDBETWEEN(1,20)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H67" s="1">
         <f t="shared" ref="H67:H126" ca="1" si="6">RANDBETWEEN(70,100)</f>
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2999,27 +2999,27 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E68" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H68" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3031,27 +3031,27 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E69" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H69" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3063,27 +3063,27 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E70" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H70" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3095,27 +3095,27 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>88</v>
       </c>
-      <c r="D71" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>62</v>
-      </c>
       <c r="E71" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G71" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H71" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3127,27 +3127,27 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E72" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="G72" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H72" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3159,27 +3159,27 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>82</v>
-      </c>
-      <c r="G73" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H73" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3191,27 +3191,27 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="E74" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G74" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H74" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3223,27 +3223,27 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E75" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="G75" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H75" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3255,27 +3255,27 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D76" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E76" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="G76" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H76" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3287,27 +3287,27 @@
       </c>
       <c r="C77" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D77" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="E77" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="G77" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H77" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3319,27 +3319,27 @@
       </c>
       <c r="C78" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D78" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="E78" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F78" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G78" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="H78" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3351,27 +3351,27 @@
       </c>
       <c r="C79" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E79" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>96</v>
       </c>
-      <c r="F79" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>78</v>
-      </c>
       <c r="G79" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H79" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3383,27 +3383,27 @@
       </c>
       <c r="C80" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E80" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G80" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H80" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3415,27 +3415,27 @@
       </c>
       <c r="C81" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E81" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="G81" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H81" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,27 +3447,27 @@
       </c>
       <c r="C82" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E82" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H82" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3479,27 +3479,27 @@
       </c>
       <c r="C83" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" ca="1" si="3"/>
         <v>93</v>
       </c>
-      <c r="D83" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="E83" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>86</v>
-      </c>
-      <c r="F83" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>83</v>
-      </c>
       <c r="G83" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H83" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3515,23 +3515,23 @@
       </c>
       <c r="D84" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E84" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="G84" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H84" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3543,27 +3543,27 @@
       </c>
       <c r="C85" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E85" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G85" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H85" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3575,27 +3575,27 @@
       </c>
       <c r="C86" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>51</v>
       </c>
-      <c r="D86" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>83</v>
-      </c>
-      <c r="E86" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>80</v>
-      </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>85</v>
-      </c>
-      <c r="G86" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="H86" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3607,27 +3607,27 @@
       </c>
       <c r="C87" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E87" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G87" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H87" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3639,27 +3639,27 @@
       </c>
       <c r="C88" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E88" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="G88" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="H88" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3671,27 +3671,27 @@
       </c>
       <c r="C89" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D89" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E89" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>97</v>
-      </c>
-      <c r="F89" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>61</v>
-      </c>
-      <c r="G89" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="H89" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3703,27 +3703,27 @@
       </c>
       <c r="C90" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D90" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E90" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="F90" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>96</v>
-      </c>
-      <c r="F90" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="G90" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="H90" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3735,27 +3735,27 @@
       </c>
       <c r="C91" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="D91" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E91" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F91" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="G91" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H91" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3767,27 +3767,27 @@
       </c>
       <c r="C92" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>51</v>
       </c>
-      <c r="D92" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>69</v>
-      </c>
       <c r="E92" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F92" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G92" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H92" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3799,27 +3799,27 @@
       </c>
       <c r="C93" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D93" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="E93" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F93" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G93" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H93" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3831,27 +3831,27 @@
       </c>
       <c r="C94" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="D94" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E94" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G94" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H94" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3863,27 +3863,27 @@
       </c>
       <c r="C95" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D95" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="E95" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="G95" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H95" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3895,27 +3895,27 @@
       </c>
       <c r="C96" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="D96" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>53</v>
       </c>
-      <c r="E96" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>68</v>
-      </c>
       <c r="F96" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="G96" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="H96" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3927,27 +3927,27 @@
       </c>
       <c r="C97" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D97" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E97" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F97" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G97" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H97" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3959,27 +3959,27 @@
       </c>
       <c r="C98" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D98" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E98" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="G98" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H98" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3991,27 +3991,27 @@
       </c>
       <c r="C99" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D99" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="E99" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G99" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H99" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4023,27 +4023,27 @@
       </c>
       <c r="C100" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D100" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E100" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="F100" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G100" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H100" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4055,27 +4055,27 @@
       </c>
       <c r="C101" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="D101" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>82</v>
       </c>
-      <c r="E101" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>83</v>
-      </c>
       <c r="F101" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="G101" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H101" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4087,27 +4087,27 @@
       </c>
       <c r="C102" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D102" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="E102" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F102" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="G102" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H102" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4119,27 +4119,27 @@
       </c>
       <c r="C103" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D103" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E103" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="F103" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G103" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H103" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4151,27 +4151,27 @@
       </c>
       <c r="C104" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="D104" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E104" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F104" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G104" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H104" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4183,27 +4183,27 @@
       </c>
       <c r="C105" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D105" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E105" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F105" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="G105" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H105" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4215,27 +4215,27 @@
       </c>
       <c r="C106" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="D106" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="E106" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F106" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G106" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H106" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4247,27 +4247,27 @@
       </c>
       <c r="C107" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D107" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E107" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F107" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G107" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H107" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4279,27 +4279,27 @@
       </c>
       <c r="C108" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D108" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E108" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="F108" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G108" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H108" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4311,27 +4311,27 @@
       </c>
       <c r="C109" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D109" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E109" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F109" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="G109" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H109" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4343,27 +4343,27 @@
       </c>
       <c r="C110" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D110" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="E110" s="1">
+        <f t="shared" ca="1" si="4"/>
         <v>84</v>
       </c>
-      <c r="E110" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>50</v>
-      </c>
       <c r="F110" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G110" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H110" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4375,27 +4375,27 @@
       </c>
       <c r="C111" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D111" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E111" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="F111" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G111" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H111" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4407,27 +4407,27 @@
       </c>
       <c r="C112" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D112" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="E112" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F112" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="G112" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="H112" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4439,27 +4439,27 @@
       </c>
       <c r="C113" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D113" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E113" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="F113" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G113" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H113" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4471,27 +4471,27 @@
       </c>
       <c r="C114" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D114" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E114" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F114" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="G114" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H114" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4507,23 +4507,23 @@
       </c>
       <c r="D115" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E115" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="F115" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="G115" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H115" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4535,27 +4535,27 @@
       </c>
       <c r="C116" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D116" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="E116" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F116" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G116" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H116" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4567,27 +4567,27 @@
       </c>
       <c r="C117" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D117" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="E117" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="F117" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="G117" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H117" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>100</v>
-      </c>
-      <c r="E117" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>81</v>
-      </c>
-      <c r="F117" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>67</v>
-      </c>
-      <c r="G117" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="H117" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>97</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4599,15 +4599,15 @@
       </c>
       <c r="C118" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="D118" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E118" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="F118" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -4615,11 +4615,11 @@
       </c>
       <c r="G118" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H118" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4631,27 +4631,27 @@
       </c>
       <c r="C119" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D119" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E119" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="F119" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G119" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H119" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4663,27 +4663,27 @@
       </c>
       <c r="C120" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D120" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="E120" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F120" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G120" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H120" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4695,27 +4695,27 @@
       </c>
       <c r="C121" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D121" s="1">
         <f t="shared" ca="1" si="4"/>
+        <v>73</v>
+      </c>
+      <c r="E121" s="1">
+        <f t="shared" ca="1" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="F121" s="1">
+        <f t="shared" ca="1" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="H121" s="1">
+        <f t="shared" ca="1" si="6"/>
         <v>80</v>
-      </c>
-      <c r="E121" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="F121" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>62</v>
-      </c>
-      <c r="G121" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="H121" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4727,15 +4727,15 @@
       </c>
       <c r="C122" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="D122" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E122" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="F122" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -4743,11 +4743,11 @@
       </c>
       <c r="G122" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H122" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4759,27 +4759,27 @@
       </c>
       <c r="C123" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D123" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E123" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F123" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="G123" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H123" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4791,27 +4791,27 @@
       </c>
       <c r="C124" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D124" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E124" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="F124" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G124" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H124" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4823,27 +4823,27 @@
       </c>
       <c r="C125" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D125" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E125" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="F125" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G125" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H125" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4855,27 +4855,27 @@
       </c>
       <c r="C126" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D126" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E126" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="F126" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G126" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H126" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>